<commit_message>
add feature to loading
create a camera switching script for lobby and loading scene
</commit_message>
<xml_diff>
--- a/timelog_ZixianLin.xlsx
+++ b/timelog_ZixianLin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linst\OneDrive\Desktop\4900 projects\chocohippo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD5D210-C79E-445E-9422-B01BD93D150D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDE6063-4A60-4A1C-8DAD-7EA62C1B5576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Zixian Lin</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>1 hour (11am - 12pm)- fixing bug with homing missle</t>
+  </si>
+  <si>
+    <t>2 hour(10:30am - 12:30pm) - creating a camera switching script for the loading and lobby scene</t>
   </si>
 </sst>
 </file>
@@ -520,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="73.28515625" defaultRowHeight="119.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1025,9 @@
       <c r="A70" s="2">
         <v>45231</v>
       </c>
-      <c r="B70" s="3"/>
+      <c r="B70" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="71" spans="1:2" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">

</xml_diff>

<commit_message>
try to fix bug
</commit_message>
<xml_diff>
--- a/timelog_ZixianLin.xlsx
+++ b/timelog_ZixianLin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linst\OneDrive\Desktop\4900 projects\chocohippo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA97F46-5587-42CF-B035-0D461AB45D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DD3216-7264-4720-99BD-6085D89407A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4395" yWindow="2250" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Zixian Lin</t>
   </si>
@@ -184,6 +184,9 @@
     <t xml:space="preserve">1 hour(9am-10am): add portal to boss3 and fixing bug with game 
 1hour(1pm-2pm): researching online on how to fix ai move
 1 hour 30 minutes (2pm -3:30pm): trying to fix the bug of AI trying to walk off the map, did not fix it yet. </t>
+  </si>
+  <si>
+    <t>1 hour(8:40pm - 9:40pm ): continue to try to fix the bug</t>
   </si>
 </sst>
 </file>
@@ -534,7 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
@@ -1060,7 +1063,9 @@
       <c r="A73" s="2">
         <v>45234</v>
       </c>
-      <c r="B73" s="3"/>
+      <c r="B73" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="74" spans="1:2" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">

</xml_diff>